<commit_message>
plus buttons and statments
</commit_message>
<xml_diff>
--- a/Webfejlesztési keretrendszerek projektmunka pontozás 2022..xlsx
+++ b/Webfejlesztési keretrendszerek projektmunka pontozás 2022..xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Peter.DESKTOP-V6T2TCT\RecipeApp\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DFCD0CEB-0EE1-4B99-8911-6B1B8A055714}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{03DD7BDE-220A-4BE4-B2F6-42DD0B0DEB95}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="51">
   <si>
     <t>Elem</t>
   </si>
@@ -176,9 +176,6 @@
   </si>
   <si>
     <t>no</t>
-  </si>
-  <si>
-    <t>Delete még nem</t>
   </si>
   <si>
     <t>Done</t>
@@ -518,7 +515,7 @@
   <dimension ref="A1:I1000"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A25" sqref="A25"/>
+      <selection activeCell="I28" sqref="I28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -627,7 +624,7 @@
         <v>13</v>
       </c>
       <c r="E8" s="13" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="9" spans="1:9" ht="12.75" x14ac:dyDescent="0.2">
@@ -641,7 +638,7 @@
         <v>15</v>
       </c>
       <c r="E9" s="13" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="10" spans="1:9" ht="26.25" x14ac:dyDescent="0.4">
@@ -697,7 +694,7 @@
         <v>4</v>
       </c>
       <c r="D13" s="13" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="14" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
@@ -742,7 +739,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="17" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A17" s="3" t="s">
         <v>29</v>
       </c>
@@ -752,8 +749,11 @@
       <c r="C17" s="5" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="18" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="G17" s="13" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A18" s="6" t="s">
         <v>31</v>
       </c>
@@ -767,7 +767,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="19" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A19" s="3" t="s">
         <v>33</v>
       </c>
@@ -781,7 +781,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="20" spans="1:5" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:7" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A20" s="6" t="s">
         <v>35</v>
       </c>
@@ -795,7 +795,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="21" spans="1:5" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:7" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A21" s="6" t="s">
         <v>37</v>
       </c>
@@ -806,7 +806,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="22" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A22" s="7" t="s">
         <v>39</v>
       </c>
@@ -815,10 +815,10 @@
         <v>40</v>
       </c>
     </row>
-    <row r="23" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A23" s="9"/>
     </row>
-    <row r="24" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A24" s="10" t="s">
         <v>40</v>
       </c>
@@ -826,28 +826,28 @@
         <v>20</v>
       </c>
     </row>
-    <row r="25" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A25" s="9"/>
     </row>
-    <row r="26" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A26" s="9"/>
     </row>
-    <row r="27" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A27" s="9"/>
     </row>
-    <row r="28" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A28" s="9"/>
     </row>
-    <row r="29" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A29" s="9"/>
     </row>
-    <row r="30" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A30" s="9"/>
     </row>
-    <row r="31" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A31" s="9"/>
     </row>
-    <row r="32" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A32" s="9"/>
     </row>
     <row r="33" spans="1:1" ht="12.75" x14ac:dyDescent="0.2">

</xml_diff>